<commit_message>
update security filter, rename orderdetails entity, rename permission
</commit_message>
<xml_diff>
--- a/src/main/resources/rawData/permissions.xlsx
+++ b/src/main/resources/rawData/permissions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Java\MyProject1\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Java\MyProject1\src\main\resources\rawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8636BADB-1638-472C-A3F4-71920ABAEF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E939A49A-953E-40F4-9530-08326AC04A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1BA804CF-1B1E-4325-A989-CFEF36273C0F}"/>
   </bookViews>
@@ -45,18 +45,12 @@
     <t>CREATE_ORDER</t>
   </si>
   <si>
-    <t>CREATE_ORDERDETAIL</t>
-  </si>
-  <si>
     <t>DELETE_PRODUCT</t>
   </si>
   <si>
     <t>DELETE_ORDER</t>
   </si>
   <si>
-    <t>DELETE_ORDERDETAIL</t>
-  </si>
-  <si>
     <t>DELETE_ACCOUNT</t>
   </si>
   <si>
@@ -69,24 +63,12 @@
     <t>UPDATE_ACCOUNT</t>
   </si>
   <si>
-    <t>CREATE_PRODUCTTYPE</t>
-  </si>
-  <si>
-    <t>CREATE_ORDERSTATUS</t>
-  </si>
-  <si>
     <t>CREATE_ROLE</t>
   </si>
   <si>
-    <t>DELETE_PRODUCTTYPE</t>
-  </si>
-  <si>
     <t>DELETE_CUSTOMER</t>
   </si>
   <si>
-    <t>DELETE_ORDERSTATUS</t>
-  </si>
-  <si>
     <t>DELETE_PERMISSION</t>
   </si>
   <si>
@@ -96,36 +78,12 @@
     <t>UPDATE_ORDER</t>
   </si>
   <si>
-    <t>UPDATE_ORDERDETAIL</t>
-  </si>
-  <si>
-    <t>UPDATE_ORDERSTATUS</t>
-  </si>
-  <si>
     <t>UPDATE_PERMISSION</t>
   </si>
   <si>
-    <t>UPDATE_PRODUCTTYPE</t>
-  </si>
-  <si>
     <t>UPDATE_ROLE</t>
   </si>
   <si>
-    <t>VIEW_ORDERSTATUS</t>
-  </si>
-  <si>
-    <t>VIEW_ACCOUNTS</t>
-  </si>
-  <si>
-    <t>VIEW_CUSTOMERS</t>
-  </si>
-  <si>
-    <t>VIEW_ORDERS</t>
-  </si>
-  <si>
-    <t>VIEW_ORDERDETAILS</t>
-  </si>
-  <si>
     <t>UPDATE_ACCOUNT_ROLE_PERMISSION</t>
   </si>
   <si>
@@ -135,19 +93,61 @@
     <t>DELETE_ACCOUNT_ROLE_PERMISSION</t>
   </si>
   <si>
-    <t>VIEW_ACCOUNT_ROLE_PERMISSIONS</t>
-  </si>
-  <si>
-    <t>VIEW_PERMISSIONS</t>
-  </si>
-  <si>
-    <t>VIEW_PRODUCTS</t>
-  </si>
-  <si>
-    <t>VIEW_PRODUCTTYPES</t>
-  </si>
-  <si>
-    <t>VIEW_ROLES</t>
+    <t>CREATE_ORDER_STATUS</t>
+  </si>
+  <si>
+    <t>CREATE_PRODUCT_TYPE</t>
+  </si>
+  <si>
+    <t>DELETE_ORDER_DETAILS</t>
+  </si>
+  <si>
+    <t>CREATE_ORDER_DETAILS</t>
+  </si>
+  <si>
+    <t>DELETE_ORDER_STATUS</t>
+  </si>
+  <si>
+    <t>DELETE_PRODUCT_TYPE</t>
+  </si>
+  <si>
+    <t>UPDATE_ORDER_DETAILS</t>
+  </si>
+  <si>
+    <t>UPDATE_ORDER_STATUS</t>
+  </si>
+  <si>
+    <t>UPDATE_PRODUCT_TYPE</t>
+  </si>
+  <si>
+    <t>VIEW_ORDER_DETAILS</t>
+  </si>
+  <si>
+    <t>VIEW_ORDER_STATUS</t>
+  </si>
+  <si>
+    <t>VIEW_ACCOUNT_ROLE_PERMISSION</t>
+  </si>
+  <si>
+    <t>VIEW_ACCOUNT</t>
+  </si>
+  <si>
+    <t>VIEW_ORDER</t>
+  </si>
+  <si>
+    <t>VIEW_CUSTOMER</t>
+  </si>
+  <si>
+    <t>VIEW_PERMISSION</t>
+  </si>
+  <si>
+    <t>VIEW_PRODUCT</t>
+  </si>
+  <si>
+    <t>VIEW_PRODUCT_TYPE</t>
+  </si>
+  <si>
+    <t>VIEW_ROLE</t>
   </si>
 </sst>
 </file>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A94A8D3-FDDC-41DD-BE88-5C78A6657F26}">
   <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -520,7 +520,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -535,12 +535,12 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -555,142 +555,142 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>